<commit_message>
#newUpdate on data read
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData.xlsx
+++ b/src/test/resources/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2520" windowWidth="13890" windowHeight="2625"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="13890" windowHeight="2625" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="capabilitiesDetails" sheetId="2" r:id="rId1"/>
@@ -67,18 +67,12 @@
     <t>CustomerUserName</t>
   </si>
   <si>
-    <t>Customerassword</t>
-  </si>
-  <si>
     <t>MaxPriceValueForFilter</t>
   </si>
   <si>
     <t>MinPriceValueForFilter</t>
   </si>
   <si>
-    <t>Invalidassword</t>
-  </si>
-  <si>
     <t>New123</t>
   </si>
   <si>
@@ -95,6 +89,12 @@
   </si>
   <si>
     <t>asd@gk.com</t>
+  </si>
+  <si>
+    <t>CustomerPassword</t>
+  </si>
+  <si>
+    <t>InvalidPassword</t>
   </si>
 </sst>
 </file>
@@ -147,16 +147,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -438,10 +432,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -452,64 +446,43 @@
     <col min="6" max="6" width="37.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
-      <c r="A1" s="3">
-        <v>0</v>
-      </c>
-      <c r="B1" s="4">
+    <row r="1" spans="1:6">
+      <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4">
+      <c r="B1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4">
+      <c r="F1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="4">
-        <v>4</v>
-      </c>
-      <c r="F1" s="4">
-        <v>5</v>
-      </c>
-      <c r="G1" s="4"/>
     </row>
-    <row r="2" spans="1:7">
-      <c r="A2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
-      <c r="A3" t="s">
+    <row r="2" spans="1:6">
+      <c r="A2" t="s">
         <v>6</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B2" t="s">
         <v>7</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C2" t="s">
         <v>11</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D2" t="s">
         <v>12</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E2" t="s">
         <v>8</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F2" t="s">
         <v>9</v>
       </c>
     </row>
@@ -521,10 +494,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -539,79 +512,56 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
-      <c r="A1" s="3">
+      <c r="A1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4">
-        <v>1</v>
-      </c>
-      <c r="C1" s="4">
-        <v>2</v>
-      </c>
-      <c r="D1" s="4">
-        <v>3</v>
-      </c>
-      <c r="E1" s="4">
-        <v>4</v>
-      </c>
-      <c r="F1" s="4">
-        <v>5</v>
-      </c>
-      <c r="G1" s="4">
-        <v>6</v>
+      <c r="E1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:7">
-      <c r="A2" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C2" s="2" t="s">
+      <c r="A2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="F2" s="2" t="s">
+      <c r="B2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" t="s">
         <v>16</v>
       </c>
-      <c r="G2" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
-      <c r="A3" s="1" t="s">
+      <c r="D2" t="s">
         <v>19</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="E2">
+        <v>8000</v>
+      </c>
+      <c r="F2">
+        <v>1000</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>21</v>
-      </c>
-      <c r="E3">
-        <v>8000</v>
-      </c>
-      <c r="F3">
-        <v>1000</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>23</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A3" r:id="rId1"/>
-    <hyperlink ref="B3" r:id="rId2"/>
-    <hyperlink ref="G3" r:id="rId3"/>
+    <hyperlink ref="A2" r:id="rId1"/>
+    <hyperlink ref="B2" r:id="rId2"/>
+    <hyperlink ref="G2" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>